<commit_message>
FIX: de popup a pestaña
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -558,22 +558,22 @@
         <v>10.8%</v>
       </c>
       <c r="W2" s="1" t="str">
+        <v>https://www.redfira.cl/</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <v>15.0%</v>
+      </c>
+      <c r="Y2" s="1" t="str">
         <v>https://www.amarillas.cl/fichas/fundacion-arturo-irarrazaval-correa_15371977</v>
       </c>
-      <c r="X2" s="1" t="str">
+      <c r="Z2" s="1" t="str">
         <v>4.8%</v>
       </c>
-      <c r="Y2" s="1" t="str">
+      <c r="AA2" s="1" t="str">
         <v>https://cl.linkedin.com/company/fundaci%C3%B3n-arturo-irarr%C3%A1zaval-correa</v>
       </c>
-      <c r="Z2" s="1" t="str">
+      <c r="AB2" s="1" t="str">
         <v>4.4%</v>
-      </c>
-      <c r="AA2" s="1" t="str">
-        <v>https://www.redfira.cl/</v>
-      </c>
-      <c r="AB2" s="1" t="str">
-        <v>15.0%</v>
       </c>
     </row>
     <row r="3">
@@ -632,34 +632,34 @@
         <v>0.0%</v>
       </c>
       <c r="S3" s="1" t="str">
-        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTA4TwNzkxNzAtNA-jTw/nombre-y-rut/IMPRENTA-GAMA-50879170-4</v>
+        <v>https://www.dgac.gob.cl/wp-content/uploads/2024/11/Lista-de-Empresas-RPA-con-AOC-y-CEO-22-NOV-2024.pdf</v>
       </c>
       <c r="T3" s="1" t="str">
         <v>0.0%</v>
       </c>
       <c r="U3" s="1" t="str">
-        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTA4TwOTU2NjAtNg-jTw/nombre-y-rut/ARREGLOS-DE-FLORES-JARDIN-ESMERALDA-50895660-6</v>
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAwTwMDkzNTAtMQ-jTw/nombre-y-rut/MENESES-Y-ROJAS-ARQUITECTOS-LIMITADA-50009350-1</v>
       </c>
       <c r="V3" s="1" t="str">
         <v>0.0%</v>
       </c>
       <c r="W3" s="1" t="str">
-        <v>https://www.dgac.gob.cl/wp-content/uploads/2024/11/Lista-de-Empresas-RPA-con-AOC-y-CEO-22-NOV-2024.pdf</v>
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAxTwNTkwODAtMA-jTw/nombre-y-rut/CELTA-50159080-0</v>
       </c>
       <c r="X3" s="1" t="str">
         <v>0.0%</v>
       </c>
       <c r="Y3" s="1" t="str">
-        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAxTwNTkwODAtMA-jTw/nombre-y-rut/CELTA-50159080-0</v>
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAzTwMTM4NjAtMw-jTw/nombre-y-rut/PHONE-BOX-PUB-LTDA.-50313860-3</v>
       </c>
       <c r="Z3" s="1" t="str">
         <v>0.0%</v>
       </c>
       <c r="AA3" s="1" t="str">
-        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAzTwMTM4NjAtMw-jTw/nombre-y-rut/PHONE-BOX-PUB-LTDA.-50313860-3</v>
+        <v>https://directorioempresaschilenas.cl/directory-bb_empresas/ubicaciones/ovalle/</v>
       </c>
       <c r="AB3" s="1" t="str">
-        <v>0.0%</v>
+        <v>16.0%</v>
       </c>
     </row>
     <row r="4">
@@ -691,13 +691,13 @@
         <v>IV REGION COQUIMBO</v>
       </c>
       <c r="J4" s="1" t="str">
-        <v>-29.9619314</v>
+        <v/>
       </c>
       <c r="K4" s="1" t="str">
-        <v>-71.2591243</v>
+        <v/>
       </c>
       <c r="L4" s="1" t="str">
-        <v>INDUSTRIAS MANUFACTURERAS METALICAS, FABRICACION DE PRODUCTOS METALICOS DE USO ESTRUCTURAL</v>
+        <v>INDUSTRIAS MANUFACTURERAS METALICAS, FAB. DE PROD. METALICOS PARA USO ESTRUCTURAL, FABRICACION DE PRODUCTOS METALICOS DE USO ESTRUCTURAL</v>
       </c>
       <c r="M4" s="1" t="str">
         <v>LINARES 569 TIERRAS BLANCAS</v>
@@ -718,34 +718,34 @@
         <v>0.0%</v>
       </c>
       <c r="S4" s="1" t="str">
-        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAwTwOTIyMTAtOQ-jTw/nombre-y-rut/MANUEL-OLAVE-E-HIJO-LTDA.-MANUEL-50092210-9</v>
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTA1TwNTYxMjAtMQ-jTw/nombre-y-rut/ALIANZA-50556120-1</v>
       </c>
       <c r="T4" s="1" t="str">
         <v>0.0%</v>
       </c>
       <c r="U4" s="1" t="str">
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTA4TwOTI1NDAtOQ-jTw/nombre-y-rut/LAZO-PONCE-ABEL-ENRIQUE-Y-OTRO-50892540-9</v>
+      </c>
+      <c r="V4" s="1" t="str">
+        <v>0.0%</v>
+      </c>
+      <c r="W4" s="1" t="str">
         <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTA2TwNDExNDAtOA-jTw/nombre-y-rut/ESTACIONAMIENTOS-MANUEL-ESPINOZA-50641140-8</v>
       </c>
-      <c r="V4" s="1" t="str">
-        <v>0.0%</v>
-      </c>
-      <c r="W4" s="1" t="str">
+      <c r="X4" s="1" t="str">
+        <v>0.0%</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <v>https://www.genealog.cl/Geneanexus/empresa/CHILE/TNTAxTwMTc2NzAtMg-jTw/nombre-y-rut/CABELLO-E-HIJO-50117670-2</v>
+      </c>
+      <c r="Z4" s="1" t="str">
+        <v>0.0%</v>
+      </c>
+      <c r="AA4" s="1" t="str">
         <v>https://www.bcn.cl/portal/resultado-busqueda?texto=Ponce%20Jorquera,%20Manuel&amp;dc_source=&amp;npagina=1&amp;orden_por=1&amp;orden_ad=desc</v>
       </c>
-      <c r="X4" s="1" t="str">
-        <v>0.0%</v>
-      </c>
-      <c r="Y4" s="1" t="str">
-        <v>https://www.linkedin.com/pub/dir/Jeremias/Ponce+Ponce</v>
-      </c>
-      <c r="Z4" s="1" t="str">
-        <v>0.0%</v>
-      </c>
-      <c r="AA4" s="1" t="str">
-        <v>https://www.ex-ante.cl/perfil-francisca-ponce-la-heredera-de-ponce-lerou-y-las-sociedades-que-ha-constituido/</v>
-      </c>
       <c r="AB4" s="1" t="str">
-        <v>6.7%</v>
+        <v>0.0%</v>
       </c>
     </row>
     <row r="5">
@@ -783,7 +783,7 @@
         <v/>
       </c>
       <c r="L5" s="1" t="str">
-        <v>Rubro HOTELES Y RESTAURANTES. Subrubro RESTAURANTES, BARES Y CANTINAS. Actividades Económicas o Giros ESTABLECIMIENTOS DE COMIDA RAPIDA (BARES, FUENTES DE SODA, GELATERIAS, PIZZERIAS Y SIMILARES). RESTAURANTES DE COMIDA RAPIDA.</v>
+        <v>La empresa 'GARCIA MARTINEZ MARIA MILAGRO Y OTRO' se dedica al rubro de HOTELES Y RESTAURANTES, específicamente en el subrubro de RESTAURANTES, BARES Y CANTINAS. Sus actividades económicas o giros incluyen ESTABLECIMIENTOS DE COMIDA RAPIDA (BARES, FUENTES DE SODA, GELATERIAS, PIZZERIAS Y SIMILARES) y RESTAURANTES DE COMIDA RAPIDA. Se encuentra en la región metropolitana, comuna de San Miguel. La empresa comenzó sus operaciones el 01/01/93 y se clasifica como una microempresa con una cantidad de personas entre 1-50.</v>
       </c>
       <c r="M5" s="1" t="str">
         <v>GRAN AVENIDA 5427</v>

</xml_diff>